<commit_message>
expanded tree data table (#21)
</commit_message>
<xml_diff>
--- a/dist/rd3stats.xlsx
+++ b/dist/rd3stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>rd3stats</t>
   </si>
@@ -24,31 +24,37 @@
     <t>RD3 Stats</t>
   </si>
   <si>
-    <t>Additional summaries and processed data (v1.0.0, 2022-06-14)</t>
+    <t>Additional summaries and processed data (v1.1.0, 2022-06-27)</t>
+  </si>
+  <si>
+    <t>treedata</t>
+  </si>
+  <si>
+    <t>Patient Tree Data</t>
+  </si>
+  <si>
+    <t>JSON stringified objects of sample-experiment links per subject</t>
+  </si>
+  <si>
+    <t>rd3stats_treedata</t>
+  </si>
+  <si>
+    <t>subjectID</t>
+  </si>
+  <si>
+    <t>familyID</t>
   </si>
   <si>
     <t>json</t>
   </si>
   <si>
-    <t>JSON Stringified data</t>
-  </si>
-  <si>
-    <t>Preprocessed JSON stringified objects for vue applications</t>
-  </si>
-  <si>
-    <t>rd3stats_json</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>identifier of the object</t>
-  </si>
-  <si>
-    <t>json stringified object</t>
+    <t>An individual who is the subject of personal data, persons to whom data refers, and from whom data are collected, processed, and stored.</t>
+  </si>
+  <si>
+    <t>A domestic group, or a number of domestic groups linked through descent (demonstrated or stipulated) from a common ancestor, marriage, or adoption.</t>
+  </si>
+  <si>
+    <t>json stringified object containing sample-experiment links</t>
   </si>
   <si>
     <t>string</t>
@@ -75,13 +81,16 @@
     <t>idAttribute</t>
   </si>
   <si>
+    <t>labelAttribute</t>
+  </si>
+  <si>
+    <t>lookupAttribute</t>
+  </si>
+  <si>
+    <t>nillable</t>
+  </si>
+  <si>
     <t>dataType</t>
-  </si>
-  <si>
-    <t>labelAttribute</t>
-  </si>
-  <si>
-    <t>lookupAttribute</t>
   </si>
 </sst>
 </file>
@@ -436,13 +445,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -471,16 +480,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -504,36 +513,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -541,22 +553,25 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -564,19 +579,42 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated model; restructured data mapping
</commit_message>
<xml_diff>
--- a/dist/rd3stats.xlsx
+++ b/dist/rd3stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>rd3stats</t>
   </si>
@@ -39,6 +39,9 @@
     <t>rd3stats_treedata</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>subjectID</t>
   </si>
   <si>
@@ -48,6 +51,9 @@
     <t>json</t>
   </si>
   <si>
+    <t>identifier of the object</t>
+  </si>
+  <si>
     <t>An individual who is the subject of personal data, persons to whom data refers, and from whom data are collected, processed, and stored.</t>
   </si>
   <si>
@@ -81,16 +87,16 @@
     <t>idAttribute</t>
   </si>
   <si>
+    <t>nillable</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
     <t>labelAttribute</t>
   </si>
   <si>
     <t>lookupAttribute</t>
-  </si>
-  <si>
-    <t>nillable</t>
-  </si>
-  <si>
-    <t>dataType</t>
   </si>
 </sst>
 </file>
@@ -445,13 +451,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -480,16 +486,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -513,7 +519,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -521,28 +527,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -553,22 +559,22 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
+      <c r="H2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -579,19 +585,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -602,19 +608,42 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>